<commit_message>
working communication with onedrive - upanddown
</commit_message>
<xml_diff>
--- a/Config/Sync.xlsx
+++ b/Config/Sync.xlsx
@@ -1,37 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dylan\2022\Nov\repo_scraper\Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A607A0-EDD4-413D-9F81-77D7C8CC82C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GIN" sheetId="1" r:id="rId1"/>
+    <sheet name="BitBucket Repos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\GIN\Applications\MODIS</t>
+  </si>
+  <si>
+    <t>MODIS</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\GIN\Applications\UTS</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>UTS2018</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Local Path</t>
+  </si>
+  <si>
+    <t>Destination Path</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\BitBucket Repos\UTS</t>
+  </si>
+  <si>
+    <t>D:\\Temp\\UTS</t>
+  </si>
+  <si>
+    <t>\\s1cn1faras14\SharedData\Temp\repo\MODIS</t>
+  </si>
+  <si>
+    <t>\\s1cn1faras14\SharedData\Temp\repo\UTS</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +135,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,82 +463,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Source</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Destination</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Trigger</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Repository</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>FEI_SHARED\Repository\GIN\Applications\MODIS</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>\\s1cn1faras14\Temp\repo\MODIS</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>MODIS</t>
-        </is>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FEI_SHARED\Repository\GIN\Applications\UTS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>\\s1cn1faras14\Temp\repo\UTS</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>UTS2018</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DF114BB7-FC4D-47FD-B19F-34B3F9D1F9E6}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{1B97937F-F305-4BAC-8499-4FFFBB78C2A0}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E0FA95-BDBD-4DA3-838A-55CFFD73DCFF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working full version, requires validation
</commit_message>
<xml_diff>
--- a/Config/Sync.xlsx
+++ b/Config/Sync.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dylan\2022\Nov\repo_scraper\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A607A0-EDD4-413D-9F81-77D7C8CC82C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F5EBCC-7732-4EE4-9BB7-AD46ADB62CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GIN" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Source</t>
   </si>
@@ -48,15 +48,9 @@
     <t>Repository</t>
   </si>
   <si>
-    <t>FEI_SHARED\Repository\GIN\Applications\MODIS</t>
-  </si>
-  <si>
     <t>MODIS</t>
   </si>
   <si>
-    <t>FEI_SHARED\Repository\GIN\Applications\UTS</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -72,16 +66,40 @@
     <t>Destination Path</t>
   </si>
   <si>
-    <t>FEI_SHARED\Repository\BitBucket Repos\UTS</t>
-  </si>
-  <si>
-    <t>D:\\Temp\\UTS</t>
-  </si>
-  <si>
     <t>\\s1cn1faras14\SharedData\Temp\repo\MODIS</t>
   </si>
   <si>
     <t>\\s1cn1faras14\SharedData\Temp\repo\UTS</t>
+  </si>
+  <si>
+    <t>Wichita_Tag_Printer</t>
+  </si>
+  <si>
+    <t>D:\\Temp\\Wichita_Tag_Printer</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\BitBucket Repos\Wichita_Tag_Printer</t>
+  </si>
+  <si>
+    <t>D:\Temp\MODIS</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\BitBucket Repos\MODIS</t>
+  </si>
+  <si>
+    <t>D:\Temp\UTS</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\Bitbucket Repos\UTS</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>\\s1cn1faras14\SharedData\Temp\repo\Wichita_Tag_Printer</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\CNH Grand Island</t>
   </si>
 </sst>
 </file>
@@ -464,16 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -493,33 +511,48 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DF114BB7-FC4D-47FD-B19F-34B3F9D1F9E6}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{1B97937F-F305-4BAC-8499-4FFFBB78C2A0}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{71A04671-40CA-4C3E-B618-BEC0C22FF8FB}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -527,10 +560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E0FA95-BDBD-4DA3-838A-55CFFD73DCFF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,24 +575,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-alpha version - working   - config not finalized
</commit_message>
<xml_diff>
--- a/Config/Sync.xlsx
+++ b/Config/Sync.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26605"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dylan\2022\Nov\repo_scraper\Config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F5EBCC-7732-4EE4-9BB7-AD46ADB62CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_333589D30CA4986804A5BD4CFD9AAA23583133FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3B89A83-B462-4EEF-9F68-2E87DB964FB3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GIN" sheetId="1" r:id="rId1"/>
-    <sheet name="BitBucket Repos" sheetId="2" r:id="rId2"/>
+    <sheet name="WICHITA" sheetId="3" r:id="rId2"/>
+    <sheet name="BitBucket Repos" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Source</t>
   </si>
@@ -48,15 +44,27 @@
     <t>Repository</t>
   </si>
   <si>
+    <t>FEI_SHARED\Repository\CNH Benson\FVS</t>
+  </si>
+  <si>
+    <t>\\s1cn1faras14\SharedData\Temp\repo\GIN</t>
+  </si>
+  <si>
     <t>MODIS</t>
   </si>
   <si>
-    <t>W</t>
+    <t>FEI_SHARED\Repository\Benson Can Cable</t>
   </si>
   <si>
     <t>UTS2018</t>
   </si>
   <si>
+    <t>\\s1cn1faras14\SharedData\Temp\repo\WICHITA</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -66,47 +74,20 @@
     <t>Destination Path</t>
   </si>
   <si>
-    <t>\\s1cn1faras14\SharedData\Temp\repo\MODIS</t>
-  </si>
-  <si>
-    <t>\\s1cn1faras14\SharedData\Temp\repo\UTS</t>
-  </si>
-  <si>
-    <t>Wichita_Tag_Printer</t>
-  </si>
-  <si>
-    <t>D:\\Temp\\Wichita_Tag_Printer</t>
-  </si>
-  <si>
-    <t>FEI_SHARED\Repository\BitBucket Repos\Wichita_Tag_Printer</t>
-  </si>
-  <si>
-    <t>D:\Temp\MODIS</t>
-  </si>
-  <si>
-    <t>FEI_SHARED\Repository\BitBucket Repos\MODIS</t>
-  </si>
-  <si>
-    <t>D:\Temp\UTS</t>
-  </si>
-  <si>
-    <t>FEI_SHARED\Repository\Bitbucket Repos\UTS</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>\\s1cn1faras14\SharedData\Temp\repo\Wichita_Tag_Printer</t>
-  </si>
-  <si>
-    <t>FEI_SHARED\Repository\CNH Grand Island</t>
+    <t>C:\Temp\Sync</t>
+  </si>
+  <si>
+    <t>FEI_SHARED\Repository\BitBucket Repos</t>
+  </si>
+  <si>
+    <t>uts2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,15 +151,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,20 +464,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,112 +492,137 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DF114BB7-FC4D-47FD-B19F-34B3F9D1F9E6}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{1B97937F-F305-4BAC-8499-4FFFBB78C2A0}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{71A04671-40CA-4C3E-B618-BEC0C22FF8FB}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E0FA95-BDBD-4DA3-838A-55CFFD73DCFF}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB78C6B2-C0CE-467E-B0F5-1C7DCF8D7508}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D63349F4-59EB-43F8-9999-2FA8B8176826}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>